<commit_message>
feat(source): allow to replace placeholders in sheet titles
</commit_message>
<xml_diff>
--- a/examples/simple/output.xlsx
+++ b/examples/simple/output.xlsx
@@ -80,6 +80,10 @@
     <font/>
     <font/>
     <font/>
+    <font>
+      <color rgb="0563C1"/>
+      <u/>
+    </font>
   </fonts>
   <fills>
     <fill>
@@ -91,8 +95,16 @@
     <fill/>
     <fill/>
     <fill/>
+    <fill/>
   </fills>
   <borders>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -130,6 +142,7 @@
     <xf fontId="1" fillId="2" borderId="1" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2"/>
     <xf fontId="2" fillId="3" borderId="2" applyFont="1" applyFill="1" applyBorder="1" numFmtId="164"/>
     <xf fontId="3" fillId="4" borderId="3" applyFont="1" applyFill="1" applyBorder="1" numFmtId="165"/>
+    <xf fontId="4" fillId="5" borderId="4" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,7 +482,7 @@
       <c r="C1" s="2">
         <v>43471</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="4">
         <v>8</v>
       </c>
       <c r="E1" t="s">

</xml_diff>

<commit_message>
fix(source): fix date formatter
Allow to user date formatter with spaces
</commit_message>
<xml_diff>
--- a/examples/simple/output.xlsx
+++ b/examples/simple/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrey/Development/xlsx-template/examples/simple/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B402C08C-255F-F742-803F-D48E56CE2DEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B8C166-18E9-7040-91B5-D8C07C56670B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="960" windowWidth="24280" windowHeight="14500" xr2:uid="{F57DA067-E5F1-5D4A-AA7E-F1E915843843}" activeTab="0"/>
   </bookViews>
@@ -54,6 +54,15 @@
     <t>date(data.dateVal)</t>
   </si>
   <si>
+    <t>number(data.numberVal 0%)</t>
+  </si>
+  <si>
+    <t>date(data.dateVal dd.mm.yyyy hh:mm)</t>
+  </si>
+  <si>
+    <t>date(data.dateVal dd.mm.yyyy)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Some String value</t>
   </si>
   <si>
@@ -67,6 +76,8 @@
   <numFmts>
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd-mm-yyyy"/>
+    <numFmt numFmtId="166" formatCode="dd.mm.yyyy hh:mm"/>
+    <numFmt numFmtId="167" formatCode="dd.mm.yyyy"/>
   </numFmts>
   <fonts x14ac:knownFonts="1">
     <font>
@@ -77,6 +88,9 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font/>
+    <font/>
+    <font/>
     <font/>
     <font/>
     <font/>
@@ -96,8 +110,32 @@
     <fill/>
     <fill/>
     <fill/>
+    <fill/>
+    <fill/>
+    <fill/>
   </fills>
   <borders>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -140,9 +178,12 @@
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="1" applyFont="1" applyFill="1" applyBorder="1" numFmtId="2"/>
-    <xf fontId="2" fillId="3" borderId="2" applyFont="1" applyFill="1" applyBorder="1" numFmtId="164"/>
-    <xf fontId="3" fillId="4" borderId="3" applyFont="1" applyFill="1" applyBorder="1" numFmtId="165"/>
-    <xf fontId="4" fillId="5" borderId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="2" fillId="3" borderId="2" applyFont="1" applyFill="1" applyBorder="1" numFmtId="9"/>
+    <xf fontId="3" fillId="4" borderId="3" applyFont="1" applyFill="1" applyBorder="1" numFmtId="164"/>
+    <xf fontId="4" fillId="5" borderId="4" applyFont="1" applyFill="1" applyBorder="1" numFmtId="165"/>
+    <xf fontId="5" fillId="6" borderId="5" applyFont="1" applyFill="1" applyBorder="1" numFmtId="166"/>
+    <xf fontId="6" fillId="7" borderId="6" applyFont="1" applyFill="1" applyBorder="1" numFmtId="167"/>
+    <xf fontId="7" fillId="8" borderId="7" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,30 +501,30 @@
   <sheetPr/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="26.83203125" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1">
         <v>3.14159</v>
       </c>
-      <c r="C1" s="2">
-        <v>43471</v>
-      </c>
-      <c r="D1" t="s" s="4">
-        <v>8</v>
+      <c r="C1" s="3">
+        <v>43471.6875</v>
+      </c>
+      <c r="D1" t="s" s="7">
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -493,8 +534,21 @@
       <c r="B2">
         <v>3.14159</v>
       </c>
-      <c r="C2" s="3">
-        <v>43471</v>
+      <c r="C2" s="4">
+        <v>43471.6875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="2">
+        <v>3.14159</v>
+      </c>
+      <c r="C3" s="5">
+        <v>43471.6875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4" s="6">
+        <v>43471.6875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>